<commit_message>
Atualização do User Stories @MassaruSueto
</commit_message>
<xml_diff>
--- a/documentacao/planilhas/userStories.xlsx
+++ b/documentacao/planilhas/userStories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laguinho zl\Documents\BandTec\2º Semestre\Projeto e Inovação\totem-monitoring\documentacao\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laguinho zl\Documents\BandTec\2º Semestre\Projeto e Inovação\totem-monitoring\documentacao\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0657E492-2935-4364-8160-80BABBF1F340}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B36149-0DE5-4974-BDBB-247ED46A3E14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t xml:space="preserve">Eu como desenvolvedor, gostaria de um site Institucional para atigir um maior público. </t>
+  </si>
+  <si>
+    <t>Eu, como funcionário de Infraestrutura, gostaria de ter acesso a gráficos para melho visulização</t>
+  </si>
+  <si>
+    <t>Eu, como desenvolvedor, gostaria de implementar DataMining para alcançar uma margem de erro mais exata</t>
+  </si>
+  <si>
+    <t>Eu, como funcionário de Infraestrutura, quero ver um histórico de funcionamento das máquinas para uma melhor administração dos Totens</t>
+  </si>
+  <si>
+    <t>Eu, como gerente, gostaria de utilizar o sistema em mais de um totem para uma melhor gestão de tempo e custos</t>
+  </si>
+  <si>
+    <t>Eu, como desenvolvedor, gostaria de fazer uma solução em Java para ter mais conforto em relação a tecnologia</t>
+  </si>
+  <si>
+    <t>Eu, como fucionário de Infraestrutura, preciso receber Logs para poder me informar sobre os incidentes</t>
   </si>
 </sst>
 </file>
@@ -135,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -146,29 +164,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -178,8 +206,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBEFEEA"/>
       <color rgb="FFA8FEE3"/>
-      <color rgb="FFBEFEEA"/>
       <color rgb="FF9CFEE0"/>
       <color rgb="FF82FED8"/>
     </mruColors>
@@ -458,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,51 +499,99 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
+      <c r="B7" s="7">
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
         <v>6</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>7</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>8</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
+        <v>10</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>